<commit_message>
Update tagging for residential houses etc.
</commit_message>
<xml_diff>
--- a/building_types.xlsx
+++ b/building_types.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nilskatla/Google Drive/Diverse/Bygninger/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Nils/Google Drive/Diverse/Bygninger/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A3DCD6B-740F-E243-9002-CE17A67A440D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E3CA6F0-C47D-244A-8D71-559C31C86CAE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="480" windowWidth="28800" windowHeight="16320" xr2:uid="{B275AFC4-266B-3244-AF4D-4C872DEED781}"/>
   </bookViews>
@@ -52,10 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="465">
-  <si>
-    <t>Kode</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="464">
   <si>
     <t>Beskrivelse</t>
   </si>
@@ -636,9 +633,6 @@
     <t>521</t>
   </si>
   <si>
-    <t>Rimelig, enkelt utstyrt overnattingssted, vanligvis serveres også mat. I byene ofte leid ut på mer fast basis; over uker, måneder eller år.</t>
-  </si>
-  <si>
     <t>Vandrer-, feriehjem</t>
   </si>
   <si>
@@ -1122,9 +1116,6 @@
     <t>Id</t>
   </si>
   <si>
-    <t xml:space="preserve">leisure=theatre </t>
-  </si>
-  <si>
     <t>amenity=community_centre</t>
   </si>
   <si>
@@ -1134,33 +1125,21 @@
     <t>amenity=social_facility</t>
   </si>
   <si>
-    <t xml:space="preserve">amenity=doctors </t>
-  </si>
-  <si>
     <t>amenity=doctors</t>
   </si>
   <si>
     <t>healthcare=yes</t>
   </si>
   <si>
-    <t xml:space="preserve">amenity=prison </t>
-  </si>
-  <si>
     <t>military=bunker</t>
   </si>
   <si>
-    <t xml:space="preserve">historic=monument </t>
-  </si>
-  <si>
     <t>amenity=social_facility + social_facility=nursing_home</t>
   </si>
   <si>
     <t>amenity=social_facility + social_facility=assisted_living</t>
   </si>
   <si>
-    <t xml:space="preserve">amenity=hospital </t>
-  </si>
-  <si>
     <t>amenity=police</t>
   </si>
   <si>
@@ -1447,6 +1426,24 @@
   </si>
   <si>
     <t>building=bungalow</t>
+  </si>
+  <si>
+    <t>Rimelig, enkelt utstyrt overnattingssted, vanligvis serveres også mat. I byene ofte leid ut på mer fast basis, over uker, måneder eller år.</t>
+  </si>
+  <si>
+    <t>amenity=hospital</t>
+  </si>
+  <si>
+    <t>historic=monument</t>
+  </si>
+  <si>
+    <t>amenity=prison</t>
+  </si>
+  <si>
+    <t>leisure=theatre</t>
+  </si>
+  <si>
+    <t>Navn</t>
   </si>
 </sst>
 </file>
@@ -1839,8 +1836,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50C66CC0-B117-2045-86F4-2FBBB4F5CB95}">
   <dimension ref="A1:E130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C98" sqref="C98"/>
+    <sheetView tabSelected="1" topLeftCell="A104" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1853,1967 +1850,1967 @@
   <sheetData>
     <row r="1" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>463</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>354</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>459</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>447</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>454</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>447</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>454</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>450</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="85" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>455</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="85" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>455</v>
+        <v>447</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="85" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>450</v>
+        <v>443</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="85" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>450</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>455</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="102" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>455</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>456</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>406</v>
+        <v>399</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>406</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>406</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>406</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>406</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>406</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>406</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>427</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>407</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>395</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>420</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="E22" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>452</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>447</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>454</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>447</v>
+      </c>
+      <c r="E24" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>454</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="E25" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>452</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>436</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="E27" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>428</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="E28" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>429</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="E29" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>430</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="E30" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>458</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="E31" s="2" t="s">
         <v>87</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>458</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="E32" s="2" t="s">
         <v>90</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>431</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>396</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="E33" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>402</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>396</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="E34" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>453</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>404</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="E35" s="2" t="s">
         <v>99</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>453</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>405</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="E36" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>431</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>396</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>397</v>
+        <v>390</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>447</v>
+        <v>440</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>453</v>
+        <v>446</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>398</v>
+        <v>391</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="E39" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>453</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>408</v>
+        <v>401</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="E41" s="2" t="s">
         <v>114</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>408</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>408</v>
+        <v>401</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>399</v>
+        <v>392</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="E43" s="2" t="s">
         <v>119</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>408</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="E44" s="2" t="s">
         <v>122</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>432</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>400</v>
+        <v>393</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="E46" s="2" t="s">
         <v>127</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>458</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>458</v>
+        <v>451</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="E48" s="2" t="s">
         <v>132</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>458</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>432</v>
+        <v>425</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A50" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="E50" s="2" t="s">
         <v>137</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>403</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="E51" s="2" t="s">
         <v>140</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>402</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>394</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="E52" s="2" t="s">
         <v>143</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>403</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="E53" s="2" t="s">
         <v>146</v>
-      </c>
-      <c r="B53" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>403</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="E54" s="2" t="s">
         <v>149</v>
-      </c>
-      <c r="B54" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>402</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>387</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="E57" s="2" t="s">
         <v>156</v>
-      </c>
-      <c r="B57" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>460</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="E58" s="2" t="s">
         <v>159</v>
-      </c>
-      <c r="B58" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>460</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>389</v>
-      </c>
-      <c r="E58" s="2" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>433</v>
+        <v>426</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>408</v>
+        <v>401</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>460</v>
+        <v>453</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>401</v>
+        <v>394</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>433</v>
+        <v>426</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>403</v>
+        <v>396</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>409</v>
+        <v>402</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>434</v>
+        <v>427</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>390</v>
+        <v>383</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="E66" s="2" t="s">
         <v>176</v>
-      </c>
-      <c r="B66" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>458</v>
-      </c>
-      <c r="E66" s="2" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A67" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="E67" s="2" t="s">
         <v>179</v>
-      </c>
-      <c r="B67" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>458</v>
-      </c>
-      <c r="E67" s="2" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>453</v>
+        <v>446</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="E69" s="2" t="s">
         <v>184</v>
-      </c>
-      <c r="B69" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>435</v>
-      </c>
-      <c r="D69" s="2" t="s">
-        <v>410</v>
-      </c>
-      <c r="E69" s="2" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A70" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="E70" s="2" t="s">
         <v>187</v>
-      </c>
-      <c r="B70" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="C70" s="2" t="s">
-        <v>435</v>
-      </c>
-      <c r="D70" s="2" t="s">
-        <v>411</v>
-      </c>
-      <c r="E70" s="2" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A71" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="E71" s="2" t="s">
         <v>190</v>
-      </c>
-      <c r="B71" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>435</v>
-      </c>
-      <c r="E71" s="2" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A72" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>435</v>
+        <v>428</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>412</v>
+        <v>405</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>194</v>
+        <v>458</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="85" x14ac:dyDescent="0.2">
       <c r="A73" s="7" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B73" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="E73" s="2" t="s">
         <v>195</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>435</v>
-      </c>
-      <c r="D73" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="E73" s="2" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A74" s="7" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B74" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="E74" s="2" t="s">
         <v>198</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>406</v>
-      </c>
-      <c r="D74" s="2" t="s">
-        <v>415</v>
-      </c>
-      <c r="E74" s="2" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="85" x14ac:dyDescent="0.2">
       <c r="A75" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B75" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="E75" s="2" t="s">
         <v>201</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>464</v>
-      </c>
-      <c r="D75" s="2" t="s">
-        <v>414</v>
-      </c>
-      <c r="E75" s="2" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A76" s="7" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B76" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="E76" s="2" t="s">
         <v>204</v>
-      </c>
-      <c r="C76" s="2" t="s">
-        <v>458</v>
-      </c>
-      <c r="E76" s="2" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A77" s="7" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B77" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="E77" s="2" t="s">
         <v>207</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>402</v>
-      </c>
-      <c r="D77" s="2" t="s">
-        <v>391</v>
-      </c>
-      <c r="E77" s="2" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A78" s="7" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B78" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="E78" s="2" t="s">
         <v>210</v>
-      </c>
-      <c r="C78" s="2" t="s">
-        <v>402</v>
-      </c>
-      <c r="E78" s="2" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A79" s="7" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B79" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="E79" s="2" t="s">
         <v>213</v>
-      </c>
-      <c r="C79" s="2" t="s">
-        <v>437</v>
-      </c>
-      <c r="D79" s="2" t="s">
-        <v>392</v>
-      </c>
-      <c r="E79" s="2" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A80" s="7" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B80" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="E80" s="2" t="s">
         <v>216</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>402</v>
-      </c>
-      <c r="E80" s="2" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A81" s="7" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B81" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="E81" s="2" t="s">
         <v>219</v>
-      </c>
-      <c r="C81" s="2" t="s">
-        <v>438</v>
-      </c>
-      <c r="D81" s="2" t="s">
-        <v>386</v>
-      </c>
-      <c r="E81" s="2" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A82" s="7" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B82" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="E82" s="2" t="s">
         <v>222</v>
-      </c>
-      <c r="C82" s="2" t="s">
-        <v>438</v>
-      </c>
-      <c r="D82" s="2" t="s">
-        <v>378</v>
-      </c>
-      <c r="E82" s="2" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A83" s="7" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B83" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="E83" s="2" t="s">
         <v>225</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>439</v>
-      </c>
-      <c r="D83" s="2" t="s">
-        <v>381</v>
-      </c>
-      <c r="E83" s="2" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A84" s="7" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B84" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="E84" s="2" t="s">
         <v>228</v>
-      </c>
-      <c r="C84" s="2" t="s">
-        <v>439</v>
-      </c>
-      <c r="D84" s="2" t="s">
-        <v>382</v>
-      </c>
-      <c r="E84" s="2" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A85" s="7" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B85" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="E85" s="2" t="s">
         <v>231</v>
-      </c>
-      <c r="C85" s="2" t="s">
-        <v>439</v>
-      </c>
-      <c r="D85" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="E85" s="2" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A86" s="7" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B86" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="E86" s="2" t="s">
         <v>234</v>
-      </c>
-      <c r="C86" s="2" t="s">
-        <v>439</v>
-      </c>
-      <c r="D86" s="2" t="s">
-        <v>383</v>
-      </c>
-      <c r="E86" s="2" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A87" s="7" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B87" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="E87" s="2" t="s">
         <v>237</v>
-      </c>
-      <c r="C87" s="2" t="s">
-        <v>439</v>
-      </c>
-      <c r="D87" s="2" t="s">
-        <v>379</v>
-      </c>
-      <c r="E87" s="2" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A88" s="7" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B88" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="E88" s="2" t="s">
         <v>240</v>
-      </c>
-      <c r="C88" s="2" t="s">
-        <v>440</v>
-      </c>
-      <c r="D88" s="2" t="s">
-        <v>380</v>
-      </c>
-      <c r="E88" s="2" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A89" s="7" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B89" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="E89" s="2" t="s">
         <v>243</v>
-      </c>
-      <c r="C89" s="2" t="s">
-        <v>403</v>
-      </c>
-      <c r="E89" s="2" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A90" s="7" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B90" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="E90" s="2" t="s">
         <v>246</v>
-      </c>
-      <c r="C90" s="2" t="s">
-        <v>440</v>
-      </c>
-      <c r="D90" s="2" t="s">
-        <v>385</v>
-      </c>
-      <c r="E90" s="2" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A91" s="7" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B91" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="E91" s="2" t="s">
         <v>249</v>
-      </c>
-      <c r="C91" s="2" t="s">
-        <v>427</v>
-      </c>
-      <c r="D91" s="2" t="s">
-        <v>373</v>
-      </c>
-      <c r="E91" s="2" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="92" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A92" s="7" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B92" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="E92" s="2" t="s">
         <v>252</v>
-      </c>
-      <c r="C92" s="2" t="s">
-        <v>427</v>
-      </c>
-      <c r="D92" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="E92" s="2" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A93" s="7" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B93" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="E93" s="2" t="s">
         <v>255</v>
-      </c>
-      <c r="C93" s="2" t="s">
-        <v>427</v>
-      </c>
-      <c r="D93" s="2" t="s">
-        <v>375</v>
-      </c>
-      <c r="E93" s="2" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A94" s="7" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B94" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="E94" s="2" t="s">
         <v>258</v>
-      </c>
-      <c r="C94" s="2" t="s">
-        <v>427</v>
-      </c>
-      <c r="E94" s="2" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A95" s="7" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B95" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="E95" s="2" t="s">
         <v>261</v>
-      </c>
-      <c r="C95" s="2" t="s">
-        <v>461</v>
-      </c>
-      <c r="D95" s="2" t="s">
-        <v>376</v>
-      </c>
-      <c r="E95" s="2" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A96" s="7" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B96" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>455</v>
+      </c>
+      <c r="E96" s="2" t="s">
         <v>264</v>
-      </c>
-      <c r="C96" s="2" t="s">
-        <v>461</v>
-      </c>
-      <c r="D96" s="2" t="s">
-        <v>462</v>
-      </c>
-      <c r="E96" s="2" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A97" s="7" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B97" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>456</v>
+      </c>
+      <c r="E97" s="2" t="s">
         <v>267</v>
-      </c>
-      <c r="C97" s="2" t="s">
-        <v>461</v>
-      </c>
-      <c r="D97" s="2" t="s">
-        <v>463</v>
-      </c>
-      <c r="E97" s="2" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A98" s="7" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B98" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="E98" s="2" t="s">
         <v>270</v>
-      </c>
-      <c r="C98" s="2" t="s">
-        <v>458</v>
-      </c>
-      <c r="E98" s="2" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="99" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A99" s="7" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B99" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="E99" s="2" t="s">
         <v>273</v>
-      </c>
-      <c r="C99" s="2" t="s">
-        <v>461</v>
-      </c>
-      <c r="D99" s="2" t="s">
-        <v>377</v>
-      </c>
-      <c r="E99" s="2" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A100" s="7" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B100" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="E100" s="2" t="s">
         <v>276</v>
-      </c>
-      <c r="C100" s="2" t="s">
-        <v>458</v>
-      </c>
-      <c r="D100" s="2" t="s">
-        <v>376</v>
-      </c>
-      <c r="E100" s="2" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="101" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A101" s="7" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B101" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>462</v>
+      </c>
+      <c r="E101" s="2" t="s">
         <v>279</v>
-      </c>
-      <c r="C101" s="2" t="s">
-        <v>427</v>
-      </c>
-      <c r="D101" s="2" t="s">
-        <v>356</v>
-      </c>
-      <c r="E101" s="2" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A102" s="7" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B102" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="D102" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="E102" s="2" t="s">
         <v>282</v>
-      </c>
-      <c r="C102" s="2" t="s">
-        <v>427</v>
-      </c>
-      <c r="D102" s="2" t="s">
-        <v>357</v>
-      </c>
-      <c r="E102" s="2" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="103" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A103" s="7" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B103" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="D103" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="E103" s="2" t="s">
         <v>285</v>
-      </c>
-      <c r="C103" s="2" t="s">
-        <v>402</v>
-      </c>
-      <c r="D103" s="2" t="s">
-        <v>372</v>
-      </c>
-      <c r="E103" s="2" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="104" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A104" s="7" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B104" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="E104" s="2" t="s">
         <v>288</v>
-      </c>
-      <c r="C104" s="2" t="s">
-        <v>427</v>
-      </c>
-      <c r="D104" s="2" t="s">
-        <v>357</v>
-      </c>
-      <c r="E104" s="2" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="105" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A105" s="7" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B105" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="D105" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="E105" s="2" t="s">
         <v>291</v>
-      </c>
-      <c r="C105" s="2" t="s">
-        <v>441</v>
-      </c>
-      <c r="D105" s="2" t="s">
-        <v>423</v>
-      </c>
-      <c r="E105" s="2" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="106" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A106" s="7" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B106" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="D106" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="E106" s="2" t="s">
         <v>294</v>
-      </c>
-      <c r="C106" s="2" t="s">
-        <v>442</v>
-      </c>
-      <c r="D106" s="2" t="s">
-        <v>424</v>
-      </c>
-      <c r="E106" s="2" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="107" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A107" s="7" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B107" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="D107" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="E107" s="2" t="s">
         <v>297</v>
-      </c>
-      <c r="C107" s="2" t="s">
-        <v>442</v>
-      </c>
-      <c r="D107" s="2" t="s">
-        <v>422</v>
-      </c>
-      <c r="E107" s="2" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="108" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A108" s="7" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B108" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="D108" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="E108" s="2" t="s">
         <v>300</v>
-      </c>
-      <c r="C108" s="2" t="s">
-        <v>441</v>
-      </c>
-      <c r="D108" s="2" t="s">
-        <v>425</v>
-      </c>
-      <c r="E108" s="2" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="109" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A109" s="7" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B109" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="D109" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="E109" s="2" t="s">
         <v>303</v>
-      </c>
-      <c r="C109" s="2" t="s">
-        <v>442</v>
-      </c>
-      <c r="D109" s="2" t="s">
-        <v>371</v>
-      </c>
-      <c r="E109" s="2" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="110" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A110" s="7" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B110" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="D110" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="E110" s="2" t="s">
         <v>306</v>
-      </c>
-      <c r="C110" s="2" t="s">
-        <v>443</v>
-      </c>
-      <c r="D110" s="2" t="s">
-        <v>426</v>
-      </c>
-      <c r="E110" s="2" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="111" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A111" s="7" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="B111" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="D111" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="E111" s="2" t="s">
         <v>309</v>
-      </c>
-      <c r="C111" s="2" t="s">
-        <v>444</v>
-      </c>
-      <c r="D111" s="2" t="s">
-        <v>368</v>
-      </c>
-      <c r="E111" s="2" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="112" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A112" s="7" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B112" s="4" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>427</v>
+        <v>420</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="E112" s="2" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="113" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A113" s="7" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B113" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="D113" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="E113" s="2" t="s">
         <v>314</v>
-      </c>
-      <c r="C113" s="2" t="s">
-        <v>427</v>
-      </c>
-      <c r="D113" s="2" t="s">
-        <v>367</v>
-      </c>
-      <c r="E113" s="2" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="114" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A114" s="7" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B114" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="D114" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="E114" s="2" t="s">
         <v>317</v>
-      </c>
-      <c r="C114" s="2" t="s">
-        <v>427</v>
-      </c>
-      <c r="D114" s="2" t="s">
-        <v>358</v>
-      </c>
-      <c r="E114" s="2" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="115" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A115" s="7" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B115" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="D115" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="E115" s="2" t="s">
         <v>320</v>
-      </c>
-      <c r="C115" s="2" t="s">
-        <v>427</v>
-      </c>
-      <c r="D115" s="5" t="s">
-        <v>359</v>
-      </c>
-      <c r="E115" s="2" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="116" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A116" s="7" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B116" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="D116" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="E116" s="2" t="s">
         <v>323</v>
-      </c>
-      <c r="C116" s="2" t="s">
-        <v>460</v>
-      </c>
-      <c r="D116" s="2" t="s">
-        <v>360</v>
-      </c>
-      <c r="E116" s="2" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="117" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A117" s="7" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B117" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="C117" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="D117" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="E117" s="2" t="s">
         <v>326</v>
-      </c>
-      <c r="C117" s="2" t="s">
-        <v>427</v>
-      </c>
-      <c r="D117" s="2" t="s">
-        <v>361</v>
-      </c>
-      <c r="E117" s="2" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="118" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A118" s="7" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B118" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="D118" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="E118" s="2" t="s">
         <v>329</v>
-      </c>
-      <c r="C118" s="2" t="s">
-        <v>427</v>
-      </c>
-      <c r="D118" s="2" t="s">
-        <v>362</v>
-      </c>
-      <c r="E118" s="2" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="119" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A119" s="7" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B119" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="C119" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="D119" s="2" t="s">
+        <v>461</v>
+      </c>
+      <c r="E119" s="2" t="s">
         <v>332</v>
-      </c>
-      <c r="C119" s="2" t="s">
-        <v>457</v>
-      </c>
-      <c r="D119" s="2" t="s">
-        <v>363</v>
-      </c>
-      <c r="E119" s="2" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="120" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A120" s="7" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B120" s="4" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>446</v>
+        <v>439</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
     </row>
     <row r="121" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A121" s="7" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B121" s="4" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>445</v>
+        <v>438</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
     </row>
     <row r="122" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A122" s="7" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B122" s="4" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>458</v>
+        <v>451</v>
       </c>
     </row>
     <row r="123" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A123" s="7" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B123" s="4" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>458</v>
+        <v>451</v>
       </c>
     </row>
     <row r="124" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A124" s="7" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="B124" s="4" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>448</v>
+        <v>441</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
     </row>
     <row r="125" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A125" s="7" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B125" s="4" t="s">
+        <v>343</v>
+      </c>
+      <c r="C125" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="E125" s="2" t="s">
         <v>345</v>
-      </c>
-      <c r="C125" s="2" t="s">
-        <v>453</v>
-      </c>
-      <c r="E125" s="2" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="126" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A126" s="7" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B126" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="C126" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="D126" s="2" t="s">
+        <v>460</v>
+      </c>
+      <c r="E126" s="2" t="s">
         <v>348</v>
-      </c>
-      <c r="C126" s="2" t="s">
-        <v>427</v>
-      </c>
-      <c r="D126" s="2" t="s">
-        <v>365</v>
-      </c>
-      <c r="E126" s="2" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="127" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A127" s="7" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B127" s="4" t="s">
+        <v>349</v>
+      </c>
+      <c r="C127" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="E127" s="2" t="s">
         <v>351</v>
-      </c>
-      <c r="C127" s="2" t="s">
-        <v>449</v>
-      </c>
-      <c r="E127" s="2" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="128" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A128" s="8" t="s">
-        <v>417</v>
+        <v>410</v>
       </c>
       <c r="B128" s="4" t="s">
-        <v>416</v>
+        <v>409</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>435</v>
+        <v>428</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>421</v>
+        <v>414</v>
       </c>
     </row>
     <row r="129" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A129" s="9" t="s">
-        <v>419</v>
+        <v>412</v>
       </c>
       <c r="B129" s="4" t="s">
-        <v>418</v>
+        <v>411</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>444</v>
+        <v>437</v>
       </c>
       <c r="D129" s="2" t="s">
-        <v>368</v>
+        <v>459</v>
       </c>
     </row>
     <row r="130" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -3821,10 +3818,10 @@
         <v>999</v>
       </c>
       <c r="B130" s="4" t="s">
+        <v>444</v>
+      </c>
+      <c r="C130" s="2" t="s">
         <v>451</v>
-      </c>
-      <c r="C130" s="2" t="s">
-        <v>458</v>
       </c>
     </row>
   </sheetData>

</xml_diff>